<commit_message>
read from file refactored for better usability
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SeleniumExamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView windowHeight="7020" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDetails" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Usernames</t>
   </si>
@@ -48,12 +48,16 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,13 +85,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -113,10 +117,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -135,10 +139,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -173,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -302,21 +306,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -333,7 +337,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -385,15 +389,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -401,8 +405,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,6 +424,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -428,6 +435,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -436,8 +446,11 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated ExcelUtils readwrite method to point to new excel file to write results
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SeleniumExamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="7020" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginDetails" r:id="rId1" sheetId="1"/>
+    <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Usernames</t>
   </si>
@@ -48,16 +48,12 @@
   </si>
   <si>
     <t>pass3</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,13 +81,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -117,10 +113,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -139,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -177,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -212,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -306,21 +302,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -337,7 +333,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -389,15 +385,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -405,8 +401,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,9 +420,6 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -435,9 +428,6 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -446,11 +436,8 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>